<commit_message>
did robustness analysis and transition prob
</commit_message>
<xml_diff>
--- a/Tables/reg_results/meanvardeps.xlsx
+++ b/Tables/reg_results/meanvardeps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Statistics\P27\IMSS\Tables\reg_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0988714-1538-4130-9E5F-B1015062D74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27737AE-DA15-4FFF-B7FB-8056216134B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27495" yWindow="-3780" windowWidth="14400" windowHeight="8175"/>
+    <workbookView xWindow="-26235" yWindow="-4890" windowWidth="21600" windowHeight="11175"/>
   </bookViews>
   <sheets>
     <sheet name="meanvardeps" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Age</t>
   </si>
@@ -38,16 +38,34 @@
   </si>
   <si>
     <t>Median lum</t>
+  </si>
+  <si>
+    <t>Formal</t>
+  </si>
+  <si>
+    <t>IMSS</t>
+  </si>
+  <si>
+    <t>Informal</t>
+  </si>
+  <si>
+    <t>No IMSS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,8 +88,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,81 +408,401 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C7"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.81640625" bestFit="true" customWidth="true"/>
+  </cols>
   <sheetData>
+    <row r="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
     <row r="2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>38.079113913176677</v>
+        <v>3.6200802887094929</v>
       </c>
       <c r="C2">
-        <v>14.810000730409991</v>
+        <v>0.31704213806515802</v>
+      </c>
+      <c r="D2">
+        <v>644996051</v>
+      </c>
+      <c r="E2">
+        <v>2579775</v>
+      </c>
+      <c r="G2">
+        <v>3.5544815888745318</v>
+      </c>
+      <c r="H2">
+        <v>0.31310039648784382</v>
+      </c>
+      <c r="I2">
+        <v>434290694</v>
+      </c>
+      <c r="J2">
+        <v>1732472</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>9.3479404467731406</v>
+        <v>2.4438638971229949</v>
       </c>
       <c r="C3">
-        <v>5.7574091535268472</v>
+        <v>0.46559967770638871</v>
+      </c>
+      <c r="D3">
+        <v>644996051</v>
+      </c>
+      <c r="E3">
+        <v>2579775</v>
+      </c>
+      <c r="G3">
+        <v>2.4049612524847599</v>
+      </c>
+      <c r="H3">
+        <v>0.44171248983115108</v>
+      </c>
+      <c r="I3">
+        <v>434290694</v>
+      </c>
+      <c r="J3">
+        <v>1732472</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>35.049542711837432</v>
+        <v>3.67389752423556</v>
       </c>
       <c r="C4">
-        <v>22.62693353130787</v>
+        <v>0.80454642286193756</v>
+      </c>
+      <c r="D4">
+        <v>644996051</v>
+      </c>
+      <c r="E4">
+        <v>2579775</v>
+      </c>
+      <c r="G4">
+        <v>3.75090407503781</v>
+      </c>
+      <c r="H4">
+        <v>0.68298447875700818</v>
+      </c>
+      <c r="I4">
+        <v>434290694</v>
+      </c>
+      <c r="J4">
+        <v>1732472</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.8751238581840459</v>
+        <v>2.4945160085192848</v>
       </c>
       <c r="C5">
-        <v>1.6572474679347391</v>
+        <v>1.586838090464729</v>
+      </c>
+      <c r="D5">
+        <v>644996051</v>
+      </c>
+      <c r="E5">
+        <v>2579775</v>
+      </c>
+      <c r="G5">
+        <v>2.5095994471525489</v>
+      </c>
+      <c r="H5">
+        <v>1.455122921004903</v>
+      </c>
+      <c r="I5">
+        <v>434290694</v>
+      </c>
+      <c r="J5">
+        <v>1732472</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>18.749833480148801</v>
+        <v>20.360934003493689</v>
       </c>
       <c r="C6">
-        <v>19.844408624330619</v>
+        <v>20.814283364912111</v>
+      </c>
+      <c r="D6">
+        <v>642867765</v>
+      </c>
+      <c r="E6">
+        <v>2564776</v>
+      </c>
+      <c r="G6">
+        <v>20.554482249681651</v>
+      </c>
+      <c r="H6">
+        <v>20.605647333456179</v>
+      </c>
+      <c r="I6">
+        <v>432808858</v>
+      </c>
+      <c r="J6">
+        <v>1722237</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>16.652435777380681</v>
+        <v>0.076338151227851203</v>
       </c>
       <c r="C7">
-        <v>21.05276804449073</v>
+        <v>0.43013425447588932</v>
+      </c>
+      <c r="D7">
+        <v>612929589</v>
+      </c>
+      <c r="E7">
+        <v>2450136</v>
+      </c>
+      <c r="G7">
+        <v>0.079810686058439301</v>
+      </c>
+      <c r="H7">
+        <v>0.4286737194574391</v>
+      </c>
+      <c r="I7">
+        <v>412315416</v>
+      </c>
+      <c r="J7">
+        <v>1643299</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>3.6200802887094929</v>
+      </c>
+      <c r="C10">
+        <v>0.31704213806515802</v>
+      </c>
+      <c r="D10">
+        <v>644996051</v>
+      </c>
+      <c r="E10">
+        <v>2579775</v>
+      </c>
+      <c r="G10">
+        <v>3.5544815888745318</v>
+      </c>
+      <c r="H10">
+        <v>0.31310039648784382</v>
+      </c>
+      <c r="I10">
+        <v>434290694</v>
+      </c>
+      <c r="J10">
+        <v>1732472</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2.4438638971229949</v>
+      </c>
+      <c r="C11">
+        <v>0.46559967770638871</v>
+      </c>
+      <c r="D11">
+        <v>644996051</v>
+      </c>
+      <c r="E11">
+        <v>2579775</v>
+      </c>
+      <c r="G11">
+        <v>2.4049612524847599</v>
+      </c>
+      <c r="H11">
+        <v>0.44171248983115108</v>
+      </c>
+      <c r="I11">
+        <v>434290694</v>
+      </c>
+      <c r="J11">
+        <v>1732472</v>
+      </c>
+    </row>
+    <row r="12" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3.67389752423556</v>
+      </c>
+      <c r="C12">
+        <v>0.80454642286193756</v>
+      </c>
+      <c r="D12">
+        <v>644996051</v>
+      </c>
+      <c r="E12">
+        <v>2579775</v>
+      </c>
+      <c r="G12">
+        <v>3.75090407503781</v>
+      </c>
+      <c r="H12">
+        <v>0.68298447875700818</v>
+      </c>
+      <c r="I12">
+        <v>434290694</v>
+      </c>
+      <c r="J12">
+        <v>1732472</v>
+      </c>
+    </row>
+    <row r="13" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>2.4945160085192848</v>
+      </c>
+      <c r="C13">
+        <v>1.586838090464729</v>
+      </c>
+      <c r="D13">
+        <v>644996051</v>
+      </c>
+      <c r="E13">
+        <v>2579775</v>
+      </c>
+      <c r="G13">
+        <v>2.5095994471525489</v>
+      </c>
+      <c r="H13">
+        <v>1.455122921004903</v>
+      </c>
+      <c r="I13">
+        <v>434290694</v>
+      </c>
+      <c r="J13">
+        <v>1732472</v>
+      </c>
+    </row>
+    <row r="14" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>20.360934003493689</v>
+      </c>
+      <c r="C14">
+        <v>20.814283364912111</v>
+      </c>
+      <c r="D14">
+        <v>642867765</v>
+      </c>
+      <c r="E14">
+        <v>2564776</v>
+      </c>
+      <c r="G14">
+        <v>20.554482249681651</v>
+      </c>
+      <c r="H14">
+        <v>20.605647333456179</v>
+      </c>
+      <c r="I14">
+        <v>432808858</v>
+      </c>
+      <c r="J14">
+        <v>1722237</v>
+      </c>
+    </row>
+    <row r="15" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>0.076338151227851203</v>
+      </c>
+      <c r="C15">
+        <v>0.43013425447588932</v>
+      </c>
+      <c r="D15">
+        <v>612929589</v>
+      </c>
+      <c r="E15">
+        <v>2450136</v>
+      </c>
+      <c r="G15">
+        <v>0.079810686058439301</v>
+      </c>
+      <c r="H15">
+        <v>0.4286737194574391</v>
+      </c>
+      <c r="I15">
+        <v>412315416</v>
+      </c>
+      <c r="J15">
+        <v>1643299</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="G9:J9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>